<commit_message>
Corregido error del step
</commit_message>
<xml_diff>
--- a/resultados_percolacion.xlsx
+++ b/resultados_percolacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="n">
-        <v>200227</v>
+        <v>839255</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.2</v>
       </c>
       <c r="B3" t="n">
-        <v>151117</v>
+        <v>631545</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.3</v>
       </c>
       <c r="B4" t="n">
-        <v>102912</v>
+        <v>429537</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.4</v>
       </c>
       <c r="B5" t="n">
-        <v>58993</v>
+        <v>245326</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.5</v>
       </c>
       <c r="B6" t="n">
-        <v>24910</v>
+        <v>102841</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.6</v>
       </c>
       <c r="B7" t="n">
-        <v>8553</v>
+        <v>35225</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.7</v>
       </c>
       <c r="B8" t="n">
-        <v>2356</v>
+        <v>9972</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.8</v>
       </c>
       <c r="B9" t="n">
-        <v>454</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.9</v>
       </c>
       <c r="B10" t="n">
-        <v>38</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11">
@@ -522,126 +522,6 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="B23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="B24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="B25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="B26" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arreglado un error de formato en el excel
</commit_message>
<xml_diff>
--- a/resultados_percolacion.xlsx
+++ b/resultados_percolacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="n">
-        <v>839255</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.2</v>
       </c>
       <c r="B3" t="n">
-        <v>631545</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.3</v>
       </c>
       <c r="B4" t="n">
-        <v>429537</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.4</v>
       </c>
       <c r="B5" t="n">
-        <v>245326</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.5</v>
       </c>
       <c r="B6" t="n">
-        <v>102841</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.6</v>
       </c>
       <c r="B7" t="n">
-        <v>35225</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.7</v>
       </c>
       <c r="B8" t="n">
-        <v>9972</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.8</v>
       </c>
       <c r="B9" t="n">
-        <v>1853</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.9</v>
       </c>
       <c r="B10" t="n">
-        <v>108</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -522,6 +522,342 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B13" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B17" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B24" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B25" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B26" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B27" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B28" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B29" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B30" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>1</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B35" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B36" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B37" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B38" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B39" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B46" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="B47" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="B48" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="B49" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B50" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Añadida percolación por nodos
</commit_message>
<xml_diff>
--- a/resultados_percolacion.xlsx
+++ b/resultados_percolacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>0.1</v>
       </c>
       <c r="B2" t="n">
-        <v>39</v>
+        <v>9830</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>0.2</v>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
+        <v>9268</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.3</v>
       </c>
       <c r="B4" t="n">
-        <v>11</v>
+        <v>8331</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>0.4</v>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>7149</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>0.5</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>5730</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.6</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>4225</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>0.7</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>0.8</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>0.9</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>962</v>
       </c>
     </row>
     <row r="11">
@@ -522,174 +522,6 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B13" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="B14" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="B15" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="B16" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B17" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="B18" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="B19" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="B20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>1</v>
-      </c>
-      <c r="B22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="B24" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="B25" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="B26" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="B27" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="B28" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="B29" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="B30" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="B31" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="B32" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>1</v>
-      </c>
-      <c r="B33" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>